<commit_message>
Refactoring hard typed code in methods
</commit_message>
<xml_diff>
--- a/export1.xlsx
+++ b/export1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stick\Documents\Python\Programs\Excel\ExcelMetrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8711C8-C0DE-40D2-BBB1-09D61E295D84}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCACAA6-A0A4-4AC8-A5FC-B38EE2807FD1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1380" windowWidth="22155" windowHeight="13800" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,20 @@
     <sheet name="Bid Breakdown_MetaData" sheetId="3" state="veryHidden" r:id="rId3"/>
     <sheet name="Bid Breakdown" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="151">
   <si>
     <t>tblAdditionalInfo</t>
   </si>
@@ -329,6 +337,9 @@
   </si>
   <si>
     <t>Bid Item</t>
+  </si>
+  <si>
+    <t>Mat Labor.</t>
   </si>
   <si>
     <t>Bid Item:  || Base Bid</t>
@@ -490,12 +501,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -510,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -524,6 +541,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1708,10 +1726,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AD49"/>
+  <dimension ref="A2:AE50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X1" sqref="A1:XFD1"/>
+      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1746,1863 +1764,1928 @@
     <col min="30" max="30" width="87.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="AE2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="2">
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="2">
         <v>6266969.3799999999</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="2">
         <v>531681.43999999994</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E3" s="3">
         <v>40397.896000000001</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F3" s="2">
         <v>2958224.5413490362</v>
       </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
         <v>4408.0010000000002</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J3" s="4">
         <v>349914.65</v>
       </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4">
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
         <v>237213.1</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N3" s="3">
         <v>2200.002</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O3" s="4">
         <v>157499.49</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P3" s="3">
         <v>47005.898999999998</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q3" s="2">
         <v>3702851.77</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R3" s="4">
         <v>620143.02</v>
       </c>
-      <c r="S2" s="4">
+      <c r="S3" s="4">
         <v>67354.19</v>
       </c>
-      <c r="T2" s="4">
+      <c r="T3" s="4">
         <v>211780.44</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U3" s="4">
         <v>668938.64</v>
       </c>
-      <c r="V2" s="4">
-        <v>0</v>
-      </c>
-      <c r="W2" s="4">
+      <c r="V3" s="4">
+        <v>0</v>
+      </c>
+      <c r="W3" s="4">
         <v>464219.87520000001</v>
       </c>
-      <c r="X2" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="X3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="7">
+        <f t="shared" ref="AE3:AE49" si="0">D3/I3</f>
+        <v>120.61735920658819</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="2">
         <v>17718.490000000002</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D4" s="2">
         <v>3697.76</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E4" s="3">
         <v>90.971999999999994</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F4" s="2">
         <v>6661.62</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I4" s="3">
         <v>29.192</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J4" s="4">
         <v>2317.3000000000002</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M4" s="4">
         <v>1570.94</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N4" s="3">
         <v>14.569000000000001</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O4" s="4">
         <v>1043.04</v>
       </c>
-      <c r="P3" s="3">
+      <c r="P4" s="3">
         <v>134.733</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q4" s="2">
         <v>11592.9</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S4" s="4">
         <v>446.05</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T4" s="4">
         <v>669.38</v>
       </c>
-      <c r="W3" s="4">
+      <c r="W4" s="4">
         <v>1312.4</v>
       </c>
-      <c r="AD3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+      <c r="AD4" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="2">
-        <v>23082.52</v>
-      </c>
-      <c r="D4" s="2">
-        <v>6102.97</v>
-      </c>
-      <c r="E4" s="3">
-        <v>73.896000000000001</v>
-      </c>
-      <c r="F4" s="2">
-        <v>5411.2</v>
-      </c>
-      <c r="I4" s="3">
-        <v>47.594000000000001</v>
-      </c>
-      <c r="J4" s="4">
-        <v>3778.11</v>
-      </c>
-      <c r="M4" s="4">
-        <v>2561.2399999999998</v>
-      </c>
-      <c r="N4" s="3">
-        <v>23.754000000000001</v>
-      </c>
-      <c r="O4" s="4">
-        <v>1700.56</v>
-      </c>
-      <c r="P4" s="3">
-        <v>145.244</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>13451.11</v>
-      </c>
-      <c r="S4" s="4">
-        <v>727.24</v>
-      </c>
-      <c r="T4" s="4">
-        <v>1091.3800000000001</v>
-      </c>
-      <c r="W4" s="4">
-        <v>1709.82</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE4" s="7">
+        <f t="shared" si="0"/>
+        <v>126.67032063579063</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C5" s="2">
-        <v>10858.15</v>
+        <v>23082.52</v>
       </c>
       <c r="D5" s="2">
-        <v>1295.49</v>
+        <v>6102.97</v>
       </c>
       <c r="E5" s="3">
-        <v>89.42</v>
+        <v>73.896000000000001</v>
       </c>
       <c r="F5" s="2">
-        <v>6547.98</v>
+        <v>5411.2</v>
       </c>
       <c r="I5" s="3">
-        <v>10.670999999999999</v>
+        <v>47.594000000000001</v>
       </c>
       <c r="J5" s="4">
-        <v>847.09</v>
+        <v>3778.11</v>
       </c>
       <c r="M5" s="4">
-        <v>574.25</v>
+        <v>2561.2399999999998</v>
       </c>
       <c r="N5" s="3">
-        <v>5.3259999999999996</v>
+        <v>23.754000000000001</v>
       </c>
       <c r="O5" s="4">
-        <v>381.28</v>
+        <v>1700.56</v>
       </c>
       <c r="P5" s="3">
-        <v>105.417</v>
+        <v>145.244</v>
       </c>
       <c r="Q5" s="2">
-        <v>8350.6</v>
+        <v>13451.11</v>
       </c>
       <c r="S5" s="4">
-        <v>163.05000000000001</v>
+        <v>727.24</v>
       </c>
       <c r="T5" s="4">
-        <v>244.7</v>
+        <v>1091.3800000000001</v>
       </c>
       <c r="W5" s="4">
-        <v>804.31</v>
+        <v>1709.82</v>
       </c>
       <c r="AD5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE5" s="7">
+        <f t="shared" si="0"/>
+        <v>128.22981888473336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>107</v>
       </c>
       <c r="C6" s="2">
-        <v>33420.730000000003</v>
+        <v>10858.15</v>
       </c>
       <c r="D6" s="2">
-        <v>2210.11</v>
+        <v>1295.49</v>
       </c>
       <c r="E6" s="3">
-        <v>336.89499999999998</v>
+        <v>89.42</v>
       </c>
       <c r="F6" s="2">
-        <v>24669.88</v>
+        <v>6547.98</v>
       </c>
       <c r="I6" s="3">
-        <v>19.625</v>
+        <v>10.670999999999999</v>
       </c>
       <c r="J6" s="4">
-        <v>1557.89</v>
+        <v>847.09</v>
       </c>
       <c r="M6" s="4">
-        <v>1056.1199999999999</v>
+        <v>574.25</v>
       </c>
       <c r="N6" s="3">
-        <v>9.7949999999999999</v>
+        <v>5.3259999999999996</v>
       </c>
       <c r="O6" s="4">
-        <v>701.22</v>
+        <v>381.28</v>
       </c>
       <c r="P6" s="3">
-        <v>366.315</v>
+        <v>105.417</v>
       </c>
       <c r="Q6" s="2">
-        <v>27985.11</v>
+        <v>8350.6</v>
       </c>
       <c r="S6" s="4">
-        <v>299.87</v>
+        <v>163.05000000000001</v>
       </c>
       <c r="T6" s="4">
-        <v>450.03</v>
+        <v>244.7</v>
       </c>
       <c r="W6" s="4">
-        <v>2475.61</v>
+        <v>804.31</v>
       </c>
       <c r="AD6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE6" s="7">
+        <f t="shared" si="0"/>
+        <v>121.40286758504358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C7" s="2">
-        <v>343502.09</v>
+        <v>33420.730000000003</v>
       </c>
       <c r="D7" s="2">
-        <v>7549.6</v>
+        <v>2210.11</v>
       </c>
       <c r="E7" s="3">
-        <v>1120.2139999999999</v>
+        <v>336.89499999999998</v>
       </c>
       <c r="F7" s="2">
-        <v>82030.13</v>
+        <v>24669.88</v>
       </c>
       <c r="I7" s="3">
-        <v>66.802999999999997</v>
+        <v>19.625</v>
       </c>
       <c r="J7" s="4">
-        <v>5302.93</v>
+        <v>1557.89</v>
       </c>
       <c r="M7" s="4">
-        <v>3594.95</v>
+        <v>1056.1199999999999</v>
       </c>
       <c r="N7" s="3">
-        <v>33.341000000000001</v>
+        <v>9.7949999999999999</v>
       </c>
       <c r="O7" s="4">
-        <v>2386.89</v>
+        <v>701.22</v>
       </c>
       <c r="P7" s="3">
-        <v>1220.3579999999999</v>
+        <v>366.315</v>
       </c>
       <c r="Q7" s="2">
-        <v>93314.9</v>
+        <v>27985.11</v>
       </c>
       <c r="S7" s="4">
-        <v>1020.75</v>
+        <v>299.87</v>
       </c>
       <c r="T7" s="4">
-        <v>1531.86</v>
-      </c>
-      <c r="U7" s="4">
-        <v>214640.38</v>
+        <v>450.03</v>
       </c>
       <c r="W7" s="4">
-        <v>25444.6</v>
+        <v>2475.61</v>
       </c>
       <c r="AD7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE7" s="7">
+        <f t="shared" si="0"/>
+        <v>112.61707006369427</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>109</v>
       </c>
       <c r="C8" s="2">
-        <v>271072.05</v>
+        <v>343502.09</v>
       </c>
       <c r="D8" s="2">
-        <v>39010.239999999998</v>
+        <v>7549.6</v>
       </c>
       <c r="E8" s="3">
-        <v>2000.989</v>
+        <v>1120.2139999999999</v>
       </c>
       <c r="F8" s="2">
-        <v>146526.81</v>
+        <v>82030.13</v>
       </c>
       <c r="I8" s="3">
-        <v>316.00099999999998</v>
+        <v>66.802999999999997</v>
       </c>
       <c r="J8" s="4">
-        <v>25084.69</v>
+        <v>5302.93</v>
       </c>
       <c r="M8" s="4">
-        <v>17005.34</v>
+        <v>3594.95</v>
       </c>
       <c r="N8" s="3">
-        <v>157.714</v>
+        <v>33.341000000000001</v>
       </c>
       <c r="O8" s="4">
-        <v>11290.83</v>
+        <v>2386.89</v>
       </c>
       <c r="P8" s="3">
-        <v>2474.7040000000002</v>
+        <v>1220.3579999999999</v>
       </c>
       <c r="Q8" s="2">
-        <v>199907.67</v>
+        <v>93314.9</v>
       </c>
       <c r="S8" s="4">
-        <v>4828.49</v>
+        <v>1020.75</v>
       </c>
       <c r="T8" s="4">
-        <v>7246.24</v>
+        <v>1531.86</v>
+      </c>
+      <c r="U8" s="4">
+        <v>214640.38</v>
       </c>
       <c r="W8" s="4">
-        <v>20079.41</v>
+        <v>25444.6</v>
       </c>
       <c r="AD8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE8" s="7">
+        <f t="shared" si="0"/>
+        <v>113.01288864272564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C9" s="2">
-        <v>2554.7399999999998</v>
+        <v>271072.05</v>
       </c>
       <c r="D9" s="2">
-        <v>179.2</v>
+        <v>39010.239999999998</v>
       </c>
       <c r="E9" s="3">
-        <v>25.396999999999998</v>
+        <v>2000.989</v>
       </c>
       <c r="F9" s="2">
-        <v>1859.75</v>
+        <v>146526.81</v>
       </c>
       <c r="I9" s="3">
-        <v>1.5760000000000001</v>
+        <v>316.00099999999998</v>
       </c>
       <c r="J9" s="4">
-        <v>125.14</v>
+        <v>25084.69</v>
       </c>
       <c r="M9" s="4">
-        <v>84.84</v>
+        <v>17005.34</v>
       </c>
       <c r="N9" s="3">
-        <v>0.78700000000000003</v>
+        <v>157.714</v>
       </c>
       <c r="O9" s="4">
-        <v>56.33</v>
+        <v>11290.83</v>
       </c>
       <c r="P9" s="3">
-        <v>27.76</v>
+        <v>2474.7040000000002</v>
       </c>
       <c r="Q9" s="2">
-        <v>2126.06</v>
+        <v>199907.67</v>
       </c>
       <c r="S9" s="4">
-        <v>24.09</v>
+        <v>4828.49</v>
       </c>
       <c r="T9" s="4">
-        <v>36.15</v>
+        <v>7246.24</v>
       </c>
       <c r="W9" s="4">
-        <v>189.24</v>
+        <v>20079.41</v>
       </c>
       <c r="AD9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE9" s="7">
+        <f t="shared" si="0"/>
+        <v>123.44973591855722</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C10" s="2">
-        <v>134628.47</v>
+        <v>2554.7399999999998</v>
       </c>
       <c r="D10" s="2">
-        <v>1797.29</v>
+        <v>179.2</v>
       </c>
       <c r="E10" s="3">
-        <v>131.52600000000001</v>
+        <v>25.396999999999998</v>
       </c>
       <c r="F10" s="2">
-        <v>9631.2800000000007</v>
+        <v>1859.75</v>
       </c>
       <c r="I10" s="3">
-        <v>14.862</v>
+        <v>1.5760000000000001</v>
       </c>
       <c r="J10" s="4">
-        <v>1179.77</v>
+        <v>125.14</v>
       </c>
       <c r="M10" s="4">
-        <v>799.79</v>
+        <v>84.84</v>
       </c>
       <c r="N10" s="3">
-        <v>7.4169999999999998</v>
+        <v>0.78700000000000003</v>
       </c>
       <c r="O10" s="4">
-        <v>531.02</v>
+        <v>56.33</v>
       </c>
       <c r="P10" s="3">
-        <v>153.80500000000001</v>
+        <v>27.76</v>
       </c>
       <c r="Q10" s="2">
-        <v>12141.86</v>
+        <v>2126.06</v>
       </c>
       <c r="S10" s="4">
-        <v>227.09</v>
+        <v>24.09</v>
       </c>
       <c r="T10" s="4">
-        <v>340.8</v>
-      </c>
-      <c r="U10" s="4">
-        <v>110148.95</v>
+        <v>36.15</v>
       </c>
       <c r="W10" s="4">
-        <v>9972.48</v>
+        <v>189.24</v>
       </c>
       <c r="AD10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE10" s="7">
+        <f t="shared" si="0"/>
+        <v>113.70558375634516</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C11" s="2">
-        <v>13088.93</v>
+        <v>134628.47</v>
       </c>
       <c r="D11" s="2">
-        <v>2852.97</v>
+        <v>1797.29</v>
       </c>
       <c r="E11" s="3">
-        <v>62.988</v>
+        <v>131.52600000000001</v>
       </c>
       <c r="F11" s="2">
-        <v>4612.43</v>
+        <v>9631.2800000000007</v>
       </c>
       <c r="I11" s="3">
-        <v>22.468</v>
+        <v>14.862</v>
       </c>
       <c r="J11" s="4">
-        <v>1783.56</v>
+        <v>1179.77</v>
       </c>
       <c r="M11" s="4">
-        <v>1209.0999999999999</v>
+        <v>799.79</v>
       </c>
       <c r="N11" s="3">
-        <v>11.214</v>
+        <v>7.4169999999999998</v>
       </c>
       <c r="O11" s="4">
-        <v>802.79</v>
+        <v>531.02</v>
       </c>
       <c r="P11" s="3">
-        <v>96.67</v>
+        <v>153.80500000000001</v>
       </c>
       <c r="Q11" s="2">
-        <v>8407.8799999999992</v>
+        <v>12141.86</v>
       </c>
       <c r="S11" s="4">
-        <v>343.31</v>
+        <v>227.09</v>
       </c>
       <c r="T11" s="4">
-        <v>515.22</v>
+        <v>340.8</v>
+      </c>
+      <c r="U11" s="4">
+        <v>110148.95</v>
       </c>
       <c r="W11" s="4">
-        <v>969.55</v>
+        <v>9972.48</v>
       </c>
       <c r="AD11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE11" s="7">
+        <f t="shared" si="0"/>
+        <v>120.93190687659803</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C12" s="2">
-        <v>507457.26</v>
+        <v>13088.93</v>
       </c>
       <c r="D12" s="2">
-        <v>80140.08</v>
+        <v>2852.97</v>
       </c>
       <c r="E12" s="3">
-        <v>3499.1930000000002</v>
+        <v>62.988</v>
       </c>
       <c r="F12" s="2">
-        <v>256236.08</v>
+        <v>4612.43</v>
       </c>
       <c r="I12" s="3">
-        <v>644.46</v>
+        <v>22.468</v>
       </c>
       <c r="J12" s="4">
-        <v>51158.31</v>
+        <v>1783.56</v>
       </c>
       <c r="M12" s="4">
-        <v>34681.089999999997</v>
+        <v>1209.0999999999999</v>
       </c>
       <c r="N12" s="3">
-        <v>321.64499999999998</v>
+        <v>11.214</v>
       </c>
       <c r="O12" s="4">
-        <v>23026.78</v>
+        <v>802.79</v>
       </c>
       <c r="P12" s="3">
-        <v>4465.2979999999998</v>
+        <v>96.67</v>
       </c>
       <c r="Q12" s="2">
-        <v>365102.26</v>
+        <v>8407.8799999999992</v>
       </c>
       <c r="S12" s="4">
-        <v>9847.34</v>
+        <v>343.31</v>
       </c>
       <c r="T12" s="4">
-        <v>14778.15</v>
+        <v>515.22</v>
       </c>
       <c r="W12" s="4">
-        <v>37589.43</v>
+        <v>969.55</v>
       </c>
       <c r="AD12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE12" s="7">
+        <f t="shared" si="0"/>
+        <v>126.97925939113405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C13" s="2">
-        <v>2926.41</v>
+        <v>507457.26</v>
       </c>
       <c r="D13" s="2">
-        <v>592.58000000000004</v>
+        <v>80140.08</v>
       </c>
       <c r="E13" s="3">
-        <v>15.654</v>
+        <v>3499.1930000000002</v>
       </c>
       <c r="F13" s="2">
-        <v>1146.3</v>
+        <v>256236.08</v>
       </c>
       <c r="I13" s="3">
-        <v>4.6870000000000003</v>
+        <v>644.46</v>
       </c>
       <c r="J13" s="4">
-        <v>372.03</v>
+        <v>51158.31</v>
       </c>
       <c r="M13" s="4">
-        <v>252.2</v>
+        <v>34681.089999999997</v>
       </c>
       <c r="N13" s="3">
-        <v>2.339</v>
+        <v>321.64499999999998</v>
       </c>
       <c r="O13" s="4">
-        <v>167.45</v>
+        <v>23026.78</v>
       </c>
       <c r="P13" s="3">
-        <v>22.68</v>
+        <v>4465.2979999999998</v>
       </c>
       <c r="Q13" s="2">
-        <v>1937.98</v>
+        <v>365102.26</v>
       </c>
       <c r="S13" s="4">
-        <v>71.61</v>
+        <v>9847.34</v>
       </c>
       <c r="T13" s="4">
-        <v>107.47</v>
+        <v>14778.15</v>
       </c>
       <c r="W13" s="4">
-        <v>216.77</v>
+        <v>37589.43</v>
       </c>
       <c r="AD13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE13" s="7">
+        <f t="shared" si="0"/>
+        <v>124.35229494460478</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C14" s="2">
-        <v>73400.100000000006</v>
+        <v>2926.41</v>
       </c>
       <c r="D14" s="2">
-        <v>15620.26</v>
+        <v>592.58000000000004</v>
       </c>
       <c r="E14" s="3">
-        <v>366.36</v>
+        <v>15.654</v>
       </c>
       <c r="F14" s="2">
-        <v>26827.51</v>
+        <v>1146.3</v>
       </c>
       <c r="I14" s="3">
-        <v>123.181</v>
+        <v>4.6870000000000003</v>
       </c>
       <c r="J14" s="4">
-        <v>9778.2800000000007</v>
+        <v>372.03</v>
       </c>
       <c r="M14" s="4">
-        <v>6628.86</v>
+        <v>252.2</v>
       </c>
       <c r="N14" s="3">
-        <v>61.478000000000002</v>
+        <v>2.339</v>
       </c>
       <c r="O14" s="4">
-        <v>4401.29</v>
+        <v>167.45</v>
       </c>
       <c r="P14" s="3">
-        <v>551.01900000000001</v>
+        <v>22.68</v>
       </c>
       <c r="Q14" s="2">
-        <v>47635.94</v>
+        <v>1937.98</v>
       </c>
       <c r="S14" s="4">
-        <v>1882.2</v>
+        <v>71.61</v>
       </c>
       <c r="T14" s="4">
-        <v>2824.66</v>
+        <v>107.47</v>
       </c>
       <c r="W14" s="4">
-        <v>5437.04</v>
+        <v>216.77</v>
       </c>
       <c r="AD14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE14" s="7">
+        <f t="shared" si="0"/>
+        <v>126.43055259227651</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>116</v>
       </c>
       <c r="C15" s="2">
-        <v>795517.43</v>
+        <v>73400.100000000006</v>
       </c>
       <c r="D15" s="2">
-        <v>102143.62</v>
+        <v>15620.26</v>
       </c>
       <c r="E15" s="3">
-        <v>5963.9960000000001</v>
+        <v>366.36</v>
       </c>
       <c r="F15" s="2">
-        <v>436726.69</v>
+        <v>26827.51</v>
       </c>
       <c r="I15" s="3">
-        <v>832.99400000000003</v>
+        <v>123.181</v>
       </c>
       <c r="J15" s="4">
-        <v>66124.479999999996</v>
+        <v>9778.2800000000007</v>
       </c>
       <c r="M15" s="4">
-        <v>44826.91</v>
+        <v>6628.86</v>
       </c>
       <c r="N15" s="3">
-        <v>415.74099999999999</v>
+        <v>61.478000000000002</v>
       </c>
       <c r="O15" s="4">
-        <v>29763.18</v>
+        <v>4401.29</v>
       </c>
       <c r="P15" s="3">
-        <v>7212.7309999999998</v>
+        <v>551.01900000000001</v>
       </c>
       <c r="Q15" s="2">
-        <v>577441.26</v>
+        <v>47635.94</v>
       </c>
       <c r="S15" s="4">
-        <v>12728.14</v>
+        <v>1882.2</v>
       </c>
       <c r="T15" s="4">
-        <v>19101.439999999999</v>
-      </c>
-      <c r="U15" s="4">
-        <v>25175.75</v>
+        <v>2824.66</v>
       </c>
       <c r="W15" s="4">
-        <v>58927.22</v>
+        <v>5437.04</v>
       </c>
       <c r="AD15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE15" s="7">
+        <f t="shared" si="0"/>
+        <v>126.80738100843475</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C16" s="2">
-        <v>25277.84</v>
+        <v>795517.43</v>
       </c>
       <c r="D16" s="2">
-        <v>3045.32</v>
+        <v>102143.62</v>
       </c>
       <c r="E16" s="3">
-        <v>207.15</v>
+        <v>5963.9960000000001</v>
       </c>
       <c r="F16" s="2">
-        <v>15169.01</v>
+        <v>436726.69</v>
       </c>
       <c r="I16" s="3">
-        <v>25.061</v>
+        <v>832.99400000000003</v>
       </c>
       <c r="J16" s="4">
-        <v>1989.39</v>
+        <v>66124.479999999996</v>
       </c>
       <c r="M16" s="4">
-        <v>1348.64</v>
+        <v>44826.91</v>
       </c>
       <c r="N16" s="3">
-        <v>12.507999999999999</v>
+        <v>415.74099999999999</v>
       </c>
       <c r="O16" s="4">
-        <v>895.44</v>
+        <v>29763.18</v>
       </c>
       <c r="P16" s="3">
-        <v>244.71899999999999</v>
+        <v>7212.7309999999998</v>
       </c>
       <c r="Q16" s="2">
-        <v>19402.48</v>
+        <v>577441.26</v>
       </c>
       <c r="S16" s="4">
-        <v>382.93</v>
+        <v>12728.14</v>
       </c>
       <c r="T16" s="4">
-        <v>574.67999999999995</v>
+        <v>19101.439999999999</v>
+      </c>
+      <c r="U16" s="4">
+        <v>25175.75</v>
       </c>
       <c r="W16" s="4">
-        <v>1872.43</v>
+        <v>58927.22</v>
       </c>
       <c r="AD16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE16" s="7">
+        <f t="shared" si="0"/>
+        <v>122.62227579070196</v>
+      </c>
+    </row>
+    <row r="17" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C17" s="2">
-        <v>118152.69</v>
+        <v>25277.84</v>
       </c>
       <c r="D17" s="2">
-        <v>17978.34</v>
+        <v>3045.32</v>
       </c>
       <c r="E17" s="3">
-        <v>838.351</v>
+        <v>207.15</v>
       </c>
       <c r="F17" s="2">
-        <v>61390.09</v>
+        <v>15169.01</v>
       </c>
       <c r="I17" s="3">
-        <v>144.98699999999999</v>
+        <v>25.061</v>
       </c>
       <c r="J17" s="4">
-        <v>11509.31</v>
+        <v>1989.39</v>
       </c>
       <c r="M17" s="4">
-        <v>7802.36</v>
+        <v>1348.64</v>
       </c>
       <c r="N17" s="3">
-        <v>72.361999999999995</v>
+        <v>12.507999999999999</v>
       </c>
       <c r="O17" s="4">
-        <v>5180.4399999999996</v>
+        <v>895.44</v>
       </c>
       <c r="P17" s="3">
-        <v>1055.7</v>
+        <v>244.71899999999999</v>
       </c>
       <c r="Q17" s="2">
-        <v>85882.2</v>
+        <v>19402.48</v>
       </c>
       <c r="S17" s="4">
-        <v>2215.4</v>
+        <v>382.93</v>
       </c>
       <c r="T17" s="4">
-        <v>3324.7</v>
+        <v>574.67999999999995</v>
       </c>
       <c r="W17" s="4">
-        <v>8752.0499999999993</v>
+        <v>1872.43</v>
       </c>
       <c r="AD17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE17" s="7">
+        <f t="shared" si="0"/>
+        <v>121.51630022744504</v>
+      </c>
+    </row>
+    <row r="18" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C18" s="2">
-        <v>1486389.63</v>
+        <v>118152.69</v>
       </c>
       <c r="D18" s="2">
-        <v>79663.69</v>
+        <v>17978.34</v>
       </c>
       <c r="E18" s="3">
-        <v>12184.232</v>
+        <v>838.351</v>
       </c>
       <c r="F18" s="2">
-        <v>892217.11</v>
+        <v>61390.09</v>
       </c>
       <c r="I18" s="3">
-        <v>707.70899999999995</v>
+        <v>144.98699999999999</v>
       </c>
       <c r="J18" s="4">
-        <v>56179.17</v>
+        <v>11509.31</v>
       </c>
       <c r="M18" s="4">
-        <v>38084.81</v>
+        <v>7802.36</v>
       </c>
       <c r="N18" s="3">
-        <v>353.21199999999999</v>
+        <v>72.361999999999995</v>
       </c>
       <c r="O18" s="4">
-        <v>25286.71</v>
+        <v>5180.4399999999996</v>
       </c>
       <c r="P18" s="3">
-        <v>13245.153</v>
+        <v>1055.7</v>
       </c>
       <c r="Q18" s="2">
-        <v>1011767.8</v>
+        <v>85882.2</v>
       </c>
       <c r="S18" s="4">
-        <v>10813.79</v>
+        <v>2215.4</v>
       </c>
       <c r="T18" s="4">
-        <v>16228.53</v>
-      </c>
-      <c r="U18" s="4">
-        <v>257812.88</v>
+        <v>3324.7</v>
       </c>
       <c r="W18" s="4">
-        <v>110102.94</v>
+        <v>8752.0499999999993</v>
       </c>
       <c r="AD18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE18" s="7">
+        <f t="shared" si="0"/>
+        <v>123.99966893583563</v>
+      </c>
+    </row>
+    <row r="19" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C19" s="2">
-        <v>154142.46</v>
+        <v>1486389.63</v>
       </c>
       <c r="D19" s="2">
-        <v>13572.81</v>
+        <v>79663.69</v>
       </c>
       <c r="E19" s="3">
-        <v>955.63900000000001</v>
+        <v>12184.232</v>
       </c>
       <c r="F19" s="2">
-        <v>69978.759999999995</v>
+        <v>892217.11</v>
       </c>
       <c r="I19" s="3">
-        <v>111.94499999999999</v>
+        <v>707.70899999999995</v>
       </c>
       <c r="J19" s="4">
-        <v>8886.39</v>
+        <v>56179.17</v>
       </c>
       <c r="M19" s="4">
-        <v>6024.23</v>
+        <v>38084.81</v>
       </c>
       <c r="N19" s="3">
-        <v>55.871000000000002</v>
+        <v>353.21199999999999</v>
       </c>
       <c r="O19" s="4">
-        <v>3999.84</v>
+        <v>25286.71</v>
       </c>
       <c r="P19" s="3">
-        <v>1123.4549999999999</v>
+        <v>13245.153</v>
       </c>
       <c r="Q19" s="2">
-        <v>88889.22</v>
+        <v>1011767.8</v>
       </c>
       <c r="S19" s="4">
-        <v>1710.52</v>
+        <v>10813.79</v>
       </c>
       <c r="T19" s="4">
-        <v>2567.02</v>
+        <v>16228.53</v>
       </c>
       <c r="U19" s="4">
-        <v>35984.93</v>
+        <v>257812.88</v>
       </c>
       <c r="W19" s="4">
-        <v>11417.96</v>
+        <v>110102.94</v>
       </c>
       <c r="AD19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE19" s="7">
+        <f t="shared" si="0"/>
+        <v>112.56560252872298</v>
+      </c>
+    </row>
+    <row r="20" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>121</v>
       </c>
       <c r="C20" s="2">
-        <v>651704.13</v>
+        <v>154142.46</v>
       </c>
       <c r="D20" s="2">
-        <v>84969.07</v>
+        <v>13572.81</v>
       </c>
       <c r="E20" s="3">
-        <v>4780.2110000000002</v>
+        <v>955.63900000000001</v>
       </c>
       <c r="F20" s="2">
-        <v>350041.44</v>
+        <v>69978.759999999995</v>
       </c>
       <c r="I20" s="3">
-        <v>691.53899999999999</v>
+        <v>111.94499999999999</v>
       </c>
       <c r="J20" s="4">
-        <v>54895.53</v>
+        <v>8886.39</v>
       </c>
       <c r="M20" s="4">
-        <v>37214.61</v>
+        <v>6024.23</v>
       </c>
       <c r="N20" s="3">
-        <v>345.142</v>
+        <v>55.871000000000002</v>
       </c>
       <c r="O20" s="4">
-        <v>24708.93</v>
+        <v>3999.84</v>
       </c>
       <c r="P20" s="3">
-        <v>5816.8919999999998</v>
+        <v>1123.4549999999999</v>
       </c>
       <c r="Q20" s="2">
-        <v>466860.51</v>
+        <v>88889.22</v>
       </c>
       <c r="S20" s="4">
-        <v>10566.7</v>
+        <v>1710.52</v>
       </c>
       <c r="T20" s="4">
-        <v>15857.72</v>
+        <v>2567.02</v>
       </c>
       <c r="U20" s="4">
-        <v>25175.75</v>
+        <v>35984.93</v>
       </c>
       <c r="W20" s="4">
-        <v>48274.38</v>
+        <v>11417.96</v>
       </c>
       <c r="AD20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE20" s="7">
+        <f t="shared" si="0"/>
+        <v>121.24534369556478</v>
+      </c>
+    </row>
+    <row r="21" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C21" s="2">
-        <v>674025.44</v>
+        <v>651704.13</v>
       </c>
       <c r="D21" s="2">
-        <v>42053.120000000003</v>
+        <v>84969.07</v>
       </c>
       <c r="E21" s="3">
-        <v>5146.9279999999999</v>
+        <v>4780.2110000000002</v>
       </c>
       <c r="F21" s="2">
-        <v>376895.09</v>
+        <v>350041.44</v>
       </c>
       <c r="I21" s="3">
-        <v>363.68700000000001</v>
+        <v>691.53899999999999</v>
       </c>
       <c r="J21" s="4">
-        <v>28870.11</v>
+        <v>54895.53</v>
       </c>
       <c r="M21" s="4">
-        <v>19571.54</v>
+        <v>37214.61</v>
       </c>
       <c r="N21" s="3">
-        <v>181.51400000000001</v>
+        <v>345.142</v>
       </c>
       <c r="O21" s="4">
-        <v>12994.68</v>
+        <v>24708.93</v>
       </c>
       <c r="P21" s="3">
-        <v>5692.1289999999999</v>
+        <v>5816.8919999999998</v>
       </c>
       <c r="Q21" s="2">
-        <v>438331.42</v>
-      </c>
-      <c r="R21" s="4">
-        <v>129816.23</v>
+        <v>466860.51</v>
       </c>
       <c r="S21" s="4">
-        <v>5557.13</v>
+        <v>10566.7</v>
       </c>
       <c r="T21" s="4">
-        <v>8339.73</v>
+        <v>15857.72</v>
+      </c>
+      <c r="U21" s="4">
+        <v>25175.75</v>
       </c>
       <c r="W21" s="4">
-        <v>49927.81</v>
+        <v>48274.38</v>
       </c>
       <c r="AD21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE21" s="7">
+        <f t="shared" si="0"/>
+        <v>122.86952724285977</v>
+      </c>
+    </row>
+    <row r="22" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C22" s="2">
-        <v>34851.06</v>
+        <v>674025.44</v>
       </c>
       <c r="D22" s="2">
-        <v>1013.06</v>
+        <v>42053.120000000003</v>
       </c>
       <c r="E22" s="3">
-        <v>144.852</v>
+        <v>5146.9279999999999</v>
       </c>
       <c r="F22" s="2">
-        <v>10607.11</v>
+        <v>376895.09</v>
       </c>
       <c r="I22" s="3">
-        <v>8.9220000000000006</v>
+        <v>363.68700000000001</v>
       </c>
       <c r="J22" s="4">
-        <v>708.24</v>
+        <v>28870.11</v>
       </c>
       <c r="M22" s="4">
-        <v>480.13</v>
+        <v>19571.54</v>
       </c>
       <c r="N22" s="3">
-        <v>4.4530000000000003</v>
+        <v>181.51400000000001</v>
       </c>
       <c r="O22" s="4">
-        <v>318.79000000000002</v>
+        <v>12994.68</v>
       </c>
       <c r="P22" s="3">
-        <v>158.227</v>
+        <v>5692.1289999999999</v>
       </c>
       <c r="Q22" s="2">
-        <v>12114.27</v>
+        <v>438331.42</v>
       </c>
       <c r="R22" s="4">
-        <v>18801.25</v>
+        <v>129816.23</v>
       </c>
       <c r="S22" s="4">
-        <v>136.33000000000001</v>
+        <v>5557.13</v>
       </c>
       <c r="T22" s="4">
-        <v>204.59</v>
+        <v>8339.73</v>
       </c>
       <c r="W22" s="4">
-        <v>2581.56</v>
+        <v>49927.81</v>
       </c>
       <c r="AD22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE22" s="7">
+        <f t="shared" si="0"/>
+        <v>115.62997852549033</v>
+      </c>
+    </row>
+    <row r="23" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>124</v>
       </c>
       <c r="C23" s="2">
-        <v>1471.74</v>
+        <v>34851.06</v>
       </c>
       <c r="D23" s="2">
-        <v>144.07</v>
+        <v>1013.06</v>
       </c>
       <c r="E23" s="3">
-        <v>13.214</v>
+        <v>144.852</v>
       </c>
       <c r="F23" s="2">
-        <v>967.62</v>
+        <v>10607.11</v>
       </c>
       <c r="I23" s="3">
-        <v>1.212</v>
+        <v>8.9220000000000006</v>
       </c>
       <c r="J23" s="4">
-        <v>96.2</v>
+        <v>708.24</v>
       </c>
       <c r="M23" s="4">
-        <v>65.22</v>
+        <v>480.13</v>
       </c>
       <c r="N23" s="3">
-        <v>0.60499999999999998</v>
+        <v>4.4530000000000003</v>
       </c>
       <c r="O23" s="4">
-        <v>43.3</v>
+        <v>318.79000000000002</v>
       </c>
       <c r="P23" s="3">
-        <v>15.031000000000001</v>
+        <v>158.227</v>
       </c>
       <c r="Q23" s="2">
-        <v>1172.3399999999999</v>
+        <v>12114.27</v>
+      </c>
+      <c r="R23" s="4">
+        <v>18801.25</v>
       </c>
       <c r="S23" s="4">
-        <v>18.52</v>
+        <v>136.33000000000001</v>
       </c>
       <c r="T23" s="4">
-        <v>27.79</v>
+        <v>204.59</v>
       </c>
       <c r="W23" s="4">
-        <v>109.02</v>
+        <v>2581.56</v>
       </c>
       <c r="AD23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE23" s="7">
+        <f t="shared" si="0"/>
+        <v>113.54629006949114</v>
+      </c>
+    </row>
+    <row r="24" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C24" s="2">
-        <v>58762.25</v>
+        <v>1471.74</v>
       </c>
       <c r="D24" s="2">
-        <v>5552.56</v>
+        <v>144.07</v>
       </c>
       <c r="E24" s="3">
-        <v>433.58300000000003</v>
+        <v>13.214</v>
       </c>
       <c r="F24" s="2">
-        <v>31750.07</v>
+        <v>967.62</v>
       </c>
       <c r="I24" s="3">
-        <v>46.125</v>
+        <v>1.212</v>
       </c>
       <c r="J24" s="4">
-        <v>3661.45</v>
+        <v>96.2</v>
       </c>
       <c r="M24" s="4">
-        <v>2482.16</v>
+        <v>65.22</v>
       </c>
       <c r="N24" s="3">
-        <v>23.02</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="O24" s="4">
-        <v>1648.05</v>
+        <v>43.3</v>
       </c>
       <c r="P24" s="3">
-        <v>502.72800000000001</v>
+        <v>15.031000000000001</v>
       </c>
       <c r="Q24" s="2">
-        <v>39541.730000000003</v>
-      </c>
-      <c r="R24" s="4">
-        <v>7552.73</v>
+        <v>1172.3399999999999</v>
       </c>
       <c r="S24" s="4">
-        <v>704.78</v>
+        <v>18.52</v>
       </c>
       <c r="T24" s="4">
-        <v>1057.69</v>
+        <v>27.79</v>
       </c>
       <c r="W24" s="4">
-        <v>4352.76</v>
+        <v>109.02</v>
       </c>
       <c r="AD24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE24" s="7">
+        <f t="shared" si="0"/>
+        <v>118.86963696369637</v>
+      </c>
+    </row>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>126</v>
       </c>
       <c r="C25" s="2">
-        <v>27436.34</v>
+        <v>58762.25</v>
       </c>
       <c r="D25" s="2">
-        <v>3523.34</v>
+        <v>5552.56</v>
       </c>
       <c r="E25" s="3">
-        <v>217.27600000000001</v>
+        <v>433.58300000000003</v>
       </c>
       <c r="F25" s="2">
-        <v>15910.51</v>
+        <v>31750.07</v>
       </c>
       <c r="I25" s="3">
-        <v>28.821999999999999</v>
+        <v>46.125</v>
       </c>
       <c r="J25" s="4">
-        <v>2287.96</v>
+        <v>3661.45</v>
       </c>
       <c r="M25" s="4">
-        <v>1551.05</v>
+        <v>2482.16</v>
       </c>
       <c r="N25" s="3">
-        <v>14.385</v>
+        <v>23.02</v>
       </c>
       <c r="O25" s="4">
-        <v>1029.83</v>
+        <v>1648.05</v>
       </c>
       <c r="P25" s="3">
-        <v>260.483</v>
+        <v>502.72800000000001</v>
       </c>
       <c r="Q25" s="2">
-        <v>20779.349999999999</v>
+        <v>39541.730000000003</v>
+      </c>
+      <c r="R25" s="4">
+        <v>7552.73</v>
       </c>
       <c r="S25" s="4">
-        <v>440.4</v>
+        <v>704.78</v>
       </c>
       <c r="T25" s="4">
-        <v>660.93</v>
+        <v>1057.69</v>
       </c>
       <c r="W25" s="4">
-        <v>2032.32</v>
+        <v>4352.76</v>
       </c>
       <c r="AD25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE25" s="7">
+        <f t="shared" si="0"/>
+        <v>120.38070460704608</v>
+      </c>
+    </row>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C26" s="2">
-        <v>6140.51</v>
+        <v>27436.34</v>
       </c>
       <c r="D26" s="2">
-        <v>1037.24</v>
+        <v>3523.34</v>
       </c>
       <c r="E26" s="3">
-        <v>40</v>
+        <v>217.27600000000001</v>
       </c>
       <c r="F26" s="2">
-        <v>2929.09</v>
+        <v>15910.51</v>
       </c>
       <c r="I26" s="3">
-        <v>8.3000000000000007</v>
+        <v>28.821999999999999</v>
       </c>
       <c r="J26" s="4">
-        <v>658.9</v>
+        <v>2287.96</v>
       </c>
       <c r="M26" s="4">
-        <v>446.68</v>
+        <v>1551.05</v>
       </c>
       <c r="N26" s="3">
-        <v>4.1429999999999998</v>
+        <v>14.385</v>
       </c>
       <c r="O26" s="4">
-        <v>296.58</v>
+        <v>1029.83</v>
       </c>
       <c r="P26" s="3">
-        <v>52.442999999999998</v>
+        <v>260.483</v>
       </c>
       <c r="Q26" s="2">
-        <v>4331.25</v>
+        <v>20779.349999999999</v>
       </c>
       <c r="S26" s="4">
-        <v>126.83</v>
+        <v>440.4</v>
       </c>
       <c r="T26" s="4">
-        <v>190.34</v>
+        <v>660.93</v>
       </c>
       <c r="W26" s="4">
-        <v>454.85</v>
+        <v>2032.32</v>
       </c>
       <c r="AD26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE26" s="7">
+        <f t="shared" si="0"/>
+        <v>122.24481299007704</v>
+      </c>
+    </row>
+    <row r="27" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C27" s="2">
-        <v>7959.05</v>
+        <v>6140.51</v>
       </c>
       <c r="D27" s="2">
-        <v>614.72</v>
+        <v>1037.24</v>
       </c>
       <c r="E27" s="3">
-        <v>77.164000000000001</v>
+        <v>40</v>
       </c>
       <c r="F27" s="2">
-        <v>5650.5</v>
+        <v>2929.09</v>
       </c>
       <c r="I27" s="3">
-        <v>5.3310000000000004</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="J27" s="4">
-        <v>423.19</v>
+        <v>658.9</v>
       </c>
       <c r="M27" s="4">
-        <v>286.89</v>
+        <v>446.68</v>
       </c>
       <c r="N27" s="3">
-        <v>2.661</v>
+        <v>4.1429999999999998</v>
       </c>
       <c r="O27" s="4">
-        <v>190.48</v>
+        <v>296.58</v>
       </c>
       <c r="P27" s="3">
-        <v>85.156000000000006</v>
+        <v>52.442999999999998</v>
       </c>
       <c r="Q27" s="2">
-        <v>6551.06</v>
+        <v>4331.25</v>
       </c>
       <c r="S27" s="4">
-        <v>81.459999999999994</v>
+        <v>126.83</v>
       </c>
       <c r="T27" s="4">
-        <v>122.25</v>
+        <v>190.34</v>
       </c>
       <c r="W27" s="4">
-        <v>589.55999999999995</v>
+        <v>454.85</v>
       </c>
       <c r="AD27" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE27" s="7">
+        <f t="shared" si="0"/>
+        <v>124.96867469879517</v>
+      </c>
+    </row>
+    <row r="28" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>129</v>
       </c>
       <c r="C28" s="2">
-        <v>35716.519999999997</v>
+        <v>7959.05</v>
       </c>
       <c r="D28" s="2">
-        <v>2840.54</v>
+        <v>614.72</v>
       </c>
       <c r="E28" s="3">
-        <v>343.43200000000002</v>
+        <v>77.164000000000001</v>
       </c>
       <c r="F28" s="2">
-        <v>25148.560000000001</v>
+        <v>5650.5</v>
       </c>
       <c r="I28" s="3">
-        <v>24.533000000000001</v>
+        <v>5.3310000000000004</v>
       </c>
       <c r="J28" s="4">
-        <v>1947.49</v>
+        <v>423.19</v>
       </c>
       <c r="M28" s="4">
-        <v>1320.24</v>
+        <v>286.89</v>
       </c>
       <c r="N28" s="3">
-        <v>12.244</v>
+        <v>2.661</v>
       </c>
       <c r="O28" s="4">
-        <v>876.58</v>
+        <v>190.48</v>
       </c>
       <c r="P28" s="3">
-        <v>380.209</v>
+        <v>85.156000000000006</v>
       </c>
       <c r="Q28" s="2">
-        <v>29292.87</v>
+        <v>6551.06</v>
       </c>
       <c r="S28" s="4">
-        <v>374.87</v>
+        <v>81.459999999999994</v>
       </c>
       <c r="T28" s="4">
-        <v>562.57000000000005</v>
+        <v>122.25</v>
       </c>
       <c r="W28" s="4">
-        <v>2645.67</v>
+        <v>589.55999999999995</v>
       </c>
       <c r="AD28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE28" s="7">
+        <f t="shared" si="0"/>
+        <v>115.3104483211405</v>
+      </c>
+    </row>
+    <row r="29" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C29" s="2">
-        <v>546218.72</v>
+        <v>35716.519999999997</v>
       </c>
       <c r="D29" s="2">
-        <v>7905.75</v>
+        <v>2840.54</v>
       </c>
       <c r="E29" s="3">
-        <v>639.95000000000005</v>
+        <v>343.43200000000002</v>
       </c>
       <c r="F29" s="2">
-        <v>46861.74</v>
+        <v>25148.560000000001</v>
       </c>
       <c r="I29" s="3">
-        <v>65.846999999999994</v>
+        <v>24.533000000000001</v>
       </c>
       <c r="J29" s="4">
-        <v>5227.01</v>
+        <v>1947.49</v>
       </c>
       <c r="M29" s="4">
-        <v>3543.48</v>
+        <v>1320.24</v>
       </c>
       <c r="N29" s="3">
-        <v>32.863999999999997</v>
+        <v>12.244</v>
       </c>
       <c r="O29" s="4">
-        <v>2352.7199999999998</v>
+        <v>876.58</v>
       </c>
       <c r="P29" s="3">
-        <v>738.66099999999994</v>
+        <v>380.209</v>
       </c>
       <c r="Q29" s="2">
-        <v>57984.95</v>
-      </c>
-      <c r="R29" s="4">
-        <v>437351.31</v>
+        <v>29292.87</v>
       </c>
       <c r="S29" s="4">
-        <v>1006.13</v>
+        <v>374.87</v>
       </c>
       <c r="T29" s="4">
-        <v>1509.93</v>
+        <v>562.57000000000005</v>
       </c>
       <c r="W29" s="4">
-        <v>40460.65</v>
+        <v>2645.67</v>
       </c>
       <c r="AD29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE29" s="7">
+        <f t="shared" si="0"/>
+        <v>115.78445359311947</v>
+      </c>
+    </row>
+    <row r="30" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C30" s="2">
-        <v>16306.67</v>
+        <v>546218.72</v>
       </c>
       <c r="D30" s="2">
-        <v>1320.44</v>
+        <v>7905.75</v>
       </c>
       <c r="E30" s="3">
-        <v>155.97900000000001</v>
+        <v>639.95000000000005</v>
       </c>
       <c r="F30" s="2">
-        <v>11421.9</v>
+        <v>46861.74</v>
       </c>
       <c r="I30" s="3">
-        <v>11.375999999999999</v>
+        <v>65.846999999999994</v>
       </c>
       <c r="J30" s="4">
-        <v>903.06</v>
+        <v>5227.01</v>
       </c>
       <c r="M30" s="4">
-        <v>612.20000000000005</v>
+        <v>3543.48</v>
       </c>
       <c r="N30" s="3">
-        <v>5.6779999999999999</v>
+        <v>32.863999999999997</v>
       </c>
       <c r="O30" s="4">
-        <v>406.47</v>
+        <v>2352.7199999999998</v>
       </c>
       <c r="P30" s="3">
-        <v>173.03299999999999</v>
+        <v>738.66099999999994</v>
       </c>
       <c r="Q30" s="2">
-        <v>13343.63</v>
+        <v>57984.95</v>
+      </c>
+      <c r="R30" s="4">
+        <v>437351.31</v>
       </c>
       <c r="S30" s="4">
-        <v>173.83</v>
+        <v>1006.13</v>
       </c>
       <c r="T30" s="4">
-        <v>260.87</v>
+        <v>1509.93</v>
       </c>
       <c r="W30" s="4">
-        <v>1207.9000000000001</v>
+        <v>40460.65</v>
       </c>
       <c r="AD30" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE30" s="7">
+        <f t="shared" si="0"/>
+        <v>120.06241742220604</v>
+      </c>
+    </row>
+    <row r="31" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C31" s="2">
-        <v>1682.46</v>
+        <v>16306.67</v>
       </c>
       <c r="D31" s="2">
-        <v>256.58</v>
+        <v>1320.44</v>
       </c>
       <c r="E31" s="3">
-        <v>11.917999999999999</v>
+        <v>155.97900000000001</v>
       </c>
       <c r="F31" s="2">
-        <v>872.72</v>
+        <v>11421.9</v>
       </c>
       <c r="I31" s="3">
-        <v>2.069</v>
+        <v>11.375999999999999</v>
       </c>
       <c r="J31" s="4">
-        <v>164.23</v>
+        <v>903.06</v>
       </c>
       <c r="M31" s="4">
-        <v>111.33</v>
+        <v>612.20000000000005</v>
       </c>
       <c r="N31" s="3">
-        <v>1.0329999999999999</v>
+        <v>5.6779999999999999</v>
       </c>
       <c r="O31" s="4">
-        <v>73.92</v>
+        <v>406.47</v>
       </c>
       <c r="P31" s="3">
-        <v>15.02</v>
+        <v>173.03299999999999</v>
       </c>
       <c r="Q31" s="2">
-        <v>1222.2</v>
+        <v>13343.63</v>
       </c>
       <c r="S31" s="4">
-        <v>31.61</v>
+        <v>173.83</v>
       </c>
       <c r="T31" s="4">
-        <v>47.44</v>
+        <v>260.87</v>
       </c>
       <c r="W31" s="4">
-        <v>124.63</v>
+        <v>1207.9000000000001</v>
       </c>
       <c r="AD31" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE31" s="7">
+        <f t="shared" si="0"/>
+        <v>116.07243319268636</v>
+      </c>
+    </row>
+    <row r="32" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C32" s="2">
-        <v>28751.22</v>
-      </c>
-      <c r="R32" s="4">
-        <v>26621.5</v>
+        <v>1682.46</v>
+      </c>
+      <c r="D32" s="2">
+        <v>256.58</v>
+      </c>
+      <c r="E32" s="3">
+        <v>11.917999999999999</v>
+      </c>
+      <c r="F32" s="2">
+        <v>872.72</v>
+      </c>
+      <c r="I32" s="3">
+        <v>2.069</v>
+      </c>
+      <c r="J32" s="4">
+        <v>164.23</v>
+      </c>
+      <c r="M32" s="4">
+        <v>111.33</v>
+      </c>
+      <c r="N32" s="3">
+        <v>1.0329999999999999</v>
+      </c>
+      <c r="O32" s="4">
+        <v>73.92</v>
+      </c>
+      <c r="P32" s="3">
+        <v>15.02</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>1222.2</v>
+      </c>
+      <c r="S32" s="4">
+        <v>31.61</v>
+      </c>
+      <c r="T32" s="4">
+        <v>47.44</v>
       </c>
       <c r="W32" s="4">
-        <v>2129.7199999999998</v>
+        <v>124.63</v>
       </c>
       <c r="AD32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE32" s="7">
+        <f t="shared" si="0"/>
+        <v>124.01159980666988</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>134</v>
       </c>
       <c r="C33" s="2">
-        <v>26898.36</v>
-      </c>
-      <c r="D33" s="2">
-        <v>1778.96</v>
-      </c>
-      <c r="E33" s="3">
-        <v>271.14100000000002</v>
-      </c>
-      <c r="F33" s="2">
-        <v>19854.89</v>
-      </c>
-      <c r="I33" s="3">
-        <v>15.795999999999999</v>
-      </c>
-      <c r="J33" s="4">
-        <v>1253.95</v>
-      </c>
-      <c r="M33" s="4">
-        <v>850.08</v>
-      </c>
-      <c r="N33" s="3">
-        <v>7.8840000000000003</v>
-      </c>
-      <c r="O33" s="4">
-        <v>564.41</v>
-      </c>
-      <c r="P33" s="3">
-        <v>294.82100000000003</v>
-      </c>
-      <c r="Q33" s="2">
-        <v>22523.33</v>
-      </c>
-      <c r="S33" s="4">
-        <v>241.37</v>
-      </c>
-      <c r="T33" s="4">
-        <v>362.23</v>
+        <v>28751.22</v>
+      </c>
+      <c r="R33" s="4">
+        <v>26621.5</v>
       </c>
       <c r="W33" s="4">
-        <v>1992.47</v>
+        <v>2129.7199999999998</v>
       </c>
       <c r="AD33" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE33" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>135</v>
       </c>
       <c r="C34" s="2">
-        <v>16298.61</v>
+        <v>26898.36</v>
       </c>
       <c r="D34" s="2">
-        <v>1219.6600000000001</v>
+        <v>1778.96</v>
       </c>
       <c r="E34" s="3">
-        <v>159.376</v>
+        <v>271.14100000000002</v>
       </c>
       <c r="F34" s="2">
-        <v>11670.66</v>
+        <v>19854.89</v>
       </c>
       <c r="I34" s="3">
-        <v>10.625999999999999</v>
+        <v>15.795999999999999</v>
       </c>
       <c r="J34" s="4">
-        <v>843.49</v>
+        <v>1253.95</v>
       </c>
       <c r="M34" s="4">
-        <v>571.82000000000005</v>
+        <v>850.08</v>
       </c>
       <c r="N34" s="3">
-        <v>5.3029999999999999</v>
+        <v>7.8840000000000003</v>
       </c>
       <c r="O34" s="4">
-        <v>379.66</v>
+        <v>564.41</v>
       </c>
       <c r="P34" s="3">
-        <v>175.30500000000001</v>
+        <v>294.82100000000003</v>
       </c>
       <c r="Q34" s="2">
-        <v>13465.63</v>
+        <v>22523.33</v>
       </c>
       <c r="S34" s="4">
-        <v>162.36000000000001</v>
+        <v>241.37</v>
       </c>
       <c r="T34" s="4">
-        <v>243.66</v>
+        <v>362.23</v>
       </c>
       <c r="W34" s="4">
-        <v>1207.3</v>
+        <v>1992.47</v>
       </c>
       <c r="AD34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="AE34" s="7">
+        <f t="shared" si="0"/>
+        <v>112.62091668776907</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>136</v>
       </c>
       <c r="C35" s="2">
+        <v>16298.61</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1219.6600000000001</v>
+      </c>
+      <c r="E35" s="3">
+        <v>159.376</v>
+      </c>
+      <c r="F35" s="2">
+        <v>11670.66</v>
+      </c>
+      <c r="I35" s="3">
+        <v>10.625999999999999</v>
+      </c>
+      <c r="J35" s="4">
+        <v>843.49</v>
+      </c>
+      <c r="M35" s="4">
+        <v>571.82000000000005</v>
+      </c>
+      <c r="N35" s="3">
+        <v>5.3029999999999999</v>
+      </c>
+      <c r="O35" s="4">
+        <v>379.66</v>
+      </c>
+      <c r="P35" s="3">
+        <v>175.30500000000001</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>13465.63</v>
+      </c>
+      <c r="S35" s="4">
+        <v>162.36000000000001</v>
+      </c>
+      <c r="T35" s="4">
+        <v>243.66</v>
+      </c>
+      <c r="W35" s="4">
+        <v>1207.3</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE35" s="7">
+        <f t="shared" si="0"/>
+        <v>114.78072651985697</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="2">
         <v>119556.31</v>
       </c>
-      <c r="T35" s="4">
+      <c r="T36" s="4">
         <v>110700.29</v>
       </c>
-      <c r="W35" s="4">
+      <c r="W36" s="4">
         <v>8856.02</v>
       </c>
-      <c r="AD35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C36" s="2">
-        <v>120.99</v>
-      </c>
-      <c r="D36" s="2">
-        <v>16.760000000000002</v>
-      </c>
-      <c r="E36" s="3">
-        <v>1.3009999999999999</v>
-      </c>
-      <c r="F36" s="2">
-        <v>95.268578549117905</v>
-      </c>
-      <c r="G36" s="3">
-        <v>0</v>
-      </c>
-      <c r="H36" s="2">
-        <v>0</v>
-      </c>
-      <c r="I36" s="3">
-        <v>0</v>
-      </c>
-      <c r="J36" s="4">
-        <v>0</v>
-      </c>
-      <c r="K36" s="3">
-        <v>0</v>
-      </c>
-      <c r="L36" s="4">
-        <v>0</v>
-      </c>
-      <c r="M36" s="4">
-        <v>0</v>
-      </c>
-      <c r="N36" s="3">
-        <v>0</v>
-      </c>
-      <c r="O36" s="4">
-        <v>0</v>
-      </c>
-      <c r="P36" s="3">
-        <v>1.3009999999999999</v>
-      </c>
-      <c r="Q36" s="2">
-        <v>95.27</v>
-      </c>
-      <c r="R36" s="4">
-        <v>0</v>
-      </c>
-      <c r="S36" s="4">
-        <v>0</v>
-      </c>
-      <c r="T36" s="4">
-        <v>0</v>
-      </c>
-      <c r="U36" s="4">
-        <v>0</v>
-      </c>
-      <c r="V36" s="4">
-        <v>0</v>
-      </c>
-      <c r="W36" s="4">
-        <v>8.9624000000000006</v>
-      </c>
-      <c r="X36" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z36" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>116</v>
+      <c r="AD36" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE36" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="C37" s="2">
         <v>120.99</v>
@@ -3614,7 +3697,34 @@
         <v>1.3009999999999999</v>
       </c>
       <c r="F37" s="2">
-        <v>95.27</v>
+        <v>95.268578549117905</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0</v>
+      </c>
+      <c r="J37" s="4">
+        <v>0</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0</v>
+      </c>
+      <c r="L37" s="4">
+        <v>0</v>
+      </c>
+      <c r="M37" s="4">
+        <v>0</v>
+      </c>
+      <c r="N37" s="3">
+        <v>0</v>
+      </c>
+      <c r="O37" s="4">
+        <v>0</v>
       </c>
       <c r="P37" s="3">
         <v>1.3009999999999999</v>
@@ -3622,90 +3732,71 @@
       <c r="Q37" s="2">
         <v>95.27</v>
       </c>
+      <c r="R37" s="4">
+        <v>0</v>
+      </c>
+      <c r="S37" s="4">
+        <v>0</v>
+      </c>
+      <c r="T37" s="4">
+        <v>0</v>
+      </c>
+      <c r="U37" s="4">
+        <v>0</v>
+      </c>
+      <c r="V37" s="4">
+        <v>0</v>
+      </c>
       <c r="W37" s="4">
+        <v>8.9624000000000006</v>
+      </c>
+      <c r="X37" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" s="2">
+        <v>120.99</v>
+      </c>
+      <c r="D38" s="2">
+        <v>16.760000000000002</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1.3009999999999999</v>
+      </c>
+      <c r="F38" s="2">
+        <v>95.27</v>
+      </c>
+      <c r="P38" s="3">
+        <v>1.3009999999999999</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>95.27</v>
+      </c>
+      <c r="W38" s="4">
         <v>8.9600000000000009</v>
       </c>
-      <c r="AD37" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="AD38" t="s">
         <v>139</v>
       </c>
-      <c r="C38" s="2">
-        <v>1011.32</v>
-      </c>
-      <c r="D38" s="2">
-        <v>124.47</v>
-      </c>
-      <c r="E38" s="3">
-        <v>11.087999999999999</v>
-      </c>
-      <c r="F38" s="2">
-        <v>811.94311987134461</v>
-      </c>
-      <c r="G38" s="3">
-        <v>0</v>
-      </c>
-      <c r="H38" s="2">
-        <v>0</v>
-      </c>
-      <c r="I38" s="3">
-        <v>0</v>
-      </c>
-      <c r="J38" s="4">
-        <v>0</v>
-      </c>
-      <c r="K38" s="3">
-        <v>0</v>
-      </c>
-      <c r="L38" s="4">
-        <v>0</v>
-      </c>
-      <c r="M38" s="4">
-        <v>0</v>
-      </c>
-      <c r="N38" s="3">
-        <v>0</v>
-      </c>
-      <c r="O38" s="4">
-        <v>0</v>
-      </c>
-      <c r="P38" s="3">
-        <v>11.087999999999999</v>
-      </c>
-      <c r="Q38" s="2">
-        <v>811.94</v>
-      </c>
-      <c r="R38" s="4">
-        <v>0</v>
-      </c>
-      <c r="S38" s="4">
-        <v>0</v>
-      </c>
-      <c r="T38" s="4">
-        <v>0</v>
-      </c>
-      <c r="U38" s="4">
-        <v>0</v>
-      </c>
-      <c r="V38" s="4">
-        <v>0</v>
-      </c>
-      <c r="W38" s="4">
-        <v>74.912800000000004</v>
-      </c>
-      <c r="X38" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z38" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
-        <v>116</v>
+      <c r="AE38" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="C39" s="2">
         <v>1011.32</v>
@@ -3717,7 +3808,34 @@
         <v>11.087999999999999</v>
       </c>
       <c r="F39" s="2">
-        <v>811.94</v>
+        <v>811.94311987134461</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0</v>
+      </c>
+      <c r="I39" s="3">
+        <v>0</v>
+      </c>
+      <c r="J39" s="4">
+        <v>0</v>
+      </c>
+      <c r="K39" s="3">
+        <v>0</v>
+      </c>
+      <c r="L39" s="4">
+        <v>0</v>
+      </c>
+      <c r="M39" s="4">
+        <v>0</v>
+      </c>
+      <c r="N39" s="3">
+        <v>0</v>
+      </c>
+      <c r="O39" s="4">
+        <v>0</v>
       </c>
       <c r="P39" s="3">
         <v>11.087999999999999</v>
@@ -3725,90 +3843,71 @@
       <c r="Q39" s="2">
         <v>811.94</v>
       </c>
+      <c r="R39" s="4">
+        <v>0</v>
+      </c>
+      <c r="S39" s="4">
+        <v>0</v>
+      </c>
+      <c r="T39" s="4">
+        <v>0</v>
+      </c>
+      <c r="U39" s="4">
+        <v>0</v>
+      </c>
+      <c r="V39" s="4">
+        <v>0</v>
+      </c>
       <c r="W39" s="4">
+        <v>74.912800000000004</v>
+      </c>
+      <c r="X39" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE39" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1011.32</v>
+      </c>
+      <c r="D40" s="2">
+        <v>124.47</v>
+      </c>
+      <c r="E40" s="3">
+        <v>11.087999999999999</v>
+      </c>
+      <c r="F40" s="2">
+        <v>811.94</v>
+      </c>
+      <c r="P40" s="3">
+        <v>11.087999999999999</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>811.94</v>
+      </c>
+      <c r="W40" s="4">
         <v>74.91</v>
       </c>
-      <c r="AD39" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="AD40" t="s">
         <v>141</v>
       </c>
-      <c r="C40" s="2">
-        <v>693.46</v>
-      </c>
-      <c r="D40" s="2">
-        <v>70.33</v>
-      </c>
-      <c r="E40" s="3">
-        <v>7.8079999999999998</v>
-      </c>
-      <c r="F40" s="2">
-        <v>571.75792568140866</v>
-      </c>
-      <c r="G40" s="3">
-        <v>0</v>
-      </c>
-      <c r="H40" s="2">
-        <v>0</v>
-      </c>
-      <c r="I40" s="3">
-        <v>0</v>
-      </c>
-      <c r="J40" s="4">
-        <v>0</v>
-      </c>
-      <c r="K40" s="3">
-        <v>0</v>
-      </c>
-      <c r="L40" s="4">
-        <v>0</v>
-      </c>
-      <c r="M40" s="4">
-        <v>0</v>
-      </c>
-      <c r="N40" s="3">
-        <v>0</v>
-      </c>
-      <c r="O40" s="4">
-        <v>0</v>
-      </c>
-      <c r="P40" s="3">
-        <v>7.8079999999999998</v>
-      </c>
-      <c r="Q40" s="2">
-        <v>571.76</v>
-      </c>
-      <c r="R40" s="4">
-        <v>0</v>
-      </c>
-      <c r="S40" s="4">
-        <v>0</v>
-      </c>
-      <c r="T40" s="4">
-        <v>0</v>
-      </c>
-      <c r="U40" s="4">
-        <v>0</v>
-      </c>
-      <c r="V40" s="4">
-        <v>0</v>
-      </c>
-      <c r="W40" s="4">
-        <v>51.367199999999997</v>
-      </c>
-      <c r="X40" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
-        <v>116</v>
+      <c r="AE40" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="C41" s="2">
         <v>693.46</v>
@@ -3820,7 +3919,34 @@
         <v>7.8079999999999998</v>
       </c>
       <c r="F41" s="2">
-        <v>571.76</v>
+        <v>571.75792568140866</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0</v>
+      </c>
+      <c r="I41" s="3">
+        <v>0</v>
+      </c>
+      <c r="J41" s="4">
+        <v>0</v>
+      </c>
+      <c r="K41" s="3">
+        <v>0</v>
+      </c>
+      <c r="L41" s="4">
+        <v>0</v>
+      </c>
+      <c r="M41" s="4">
+        <v>0</v>
+      </c>
+      <c r="N41" s="3">
+        <v>0</v>
+      </c>
+      <c r="O41" s="4">
+        <v>0</v>
       </c>
       <c r="P41" s="3">
         <v>7.8079999999999998</v>
@@ -3828,90 +3954,71 @@
       <c r="Q41" s="2">
         <v>571.76</v>
       </c>
+      <c r="R41" s="4">
+        <v>0</v>
+      </c>
+      <c r="S41" s="4">
+        <v>0</v>
+      </c>
+      <c r="T41" s="4">
+        <v>0</v>
+      </c>
+      <c r="U41" s="4">
+        <v>0</v>
+      </c>
+      <c r="V41" s="4">
+        <v>0</v>
+      </c>
       <c r="W41" s="4">
+        <v>51.367199999999997</v>
+      </c>
+      <c r="X41" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE41" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="2">
+        <v>693.46</v>
+      </c>
+      <c r="D42" s="2">
+        <v>70.33</v>
+      </c>
+      <c r="E42" s="3">
+        <v>7.8079999999999998</v>
+      </c>
+      <c r="F42" s="2">
+        <v>571.76</v>
+      </c>
+      <c r="P42" s="3">
+        <v>7.8079999999999998</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>571.76</v>
+      </c>
+      <c r="W42" s="4">
         <v>51.37</v>
       </c>
-      <c r="AD41" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="AD42" t="s">
         <v>143</v>
       </c>
-      <c r="C42" s="2">
-        <v>-35678.730000000003</v>
-      </c>
-      <c r="D42" s="2">
-        <v>5591.26</v>
-      </c>
-      <c r="E42" s="3">
-        <v>-527.49699999999996</v>
-      </c>
-      <c r="F42" s="2">
-        <v>-38627.124810856301</v>
-      </c>
-      <c r="G42" s="3">
-        <v>0</v>
-      </c>
-      <c r="H42" s="2">
-        <v>0</v>
-      </c>
-      <c r="I42" s="3">
-        <v>0</v>
-      </c>
-      <c r="J42" s="4">
-        <v>0</v>
-      </c>
-      <c r="K42" s="3">
-        <v>0</v>
-      </c>
-      <c r="L42" s="4">
-        <v>0</v>
-      </c>
-      <c r="M42" s="4">
-        <v>0</v>
-      </c>
-      <c r="N42" s="3">
-        <v>0</v>
-      </c>
-      <c r="O42" s="4">
-        <v>0</v>
-      </c>
-      <c r="P42" s="3">
-        <v>-527.49699999999996</v>
-      </c>
-      <c r="Q42" s="2">
-        <v>-38627.120000000003</v>
-      </c>
-      <c r="R42" s="4">
-        <v>0</v>
-      </c>
-      <c r="S42" s="4">
-        <v>0</v>
-      </c>
-      <c r="T42" s="4">
-        <v>0</v>
-      </c>
-      <c r="U42" s="4">
-        <v>0</v>
-      </c>
-      <c r="V42" s="4">
-        <v>0</v>
-      </c>
-      <c r="W42" s="4">
-        <v>-2642.8688000000002</v>
-      </c>
-      <c r="X42" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z42" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
-        <v>109</v>
+      <c r="AE42" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="C43" s="2">
         <v>-35678.730000000003</v>
@@ -3923,7 +4030,34 @@
         <v>-527.49699999999996</v>
       </c>
       <c r="F43" s="2">
-        <v>-38627.120000000003</v>
+        <v>-38627.124810856301</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3">
+        <v>0</v>
+      </c>
+      <c r="J43" s="4">
+        <v>0</v>
+      </c>
+      <c r="K43" s="3">
+        <v>0</v>
+      </c>
+      <c r="L43" s="4">
+        <v>0</v>
+      </c>
+      <c r="M43" s="4">
+        <v>0</v>
+      </c>
+      <c r="N43" s="3">
+        <v>0</v>
+      </c>
+      <c r="O43" s="4">
+        <v>0</v>
       </c>
       <c r="P43" s="3">
         <v>-527.49699999999996</v>
@@ -3931,222 +4065,215 @@
       <c r="Q43" s="2">
         <v>-38627.120000000003</v>
       </c>
+      <c r="R43" s="4">
+        <v>0</v>
+      </c>
+      <c r="S43" s="4">
+        <v>0</v>
+      </c>
+      <c r="T43" s="4">
+        <v>0</v>
+      </c>
+      <c r="U43" s="4">
+        <v>0</v>
+      </c>
+      <c r="V43" s="4">
+        <v>0</v>
+      </c>
       <c r="W43" s="4">
+        <v>-2642.8688000000002</v>
+      </c>
+      <c r="X43" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" s="2">
+        <v>-35678.730000000003</v>
+      </c>
+      <c r="D44" s="2">
+        <v>5591.26</v>
+      </c>
+      <c r="E44" s="3">
+        <v>-527.49699999999996</v>
+      </c>
+      <c r="F44" s="2">
+        <v>-38627.120000000003</v>
+      </c>
+      <c r="P44" s="3">
+        <v>-527.49699999999996</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>-38627.120000000003</v>
+      </c>
+      <c r="W44" s="4">
         <v>-2642.87</v>
       </c>
-      <c r="AD43" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="AD44" t="s">
         <v>145</v>
       </c>
-      <c r="C44" s="2">
+      <c r="AE44" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" s="2">
         <v>135355.04</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D45" s="2">
         <v>-27678.080000000002</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E45" s="3">
         <v>2089.4810000000002</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F45" s="2">
         <v>153006.82918938459</v>
       </c>
-      <c r="G44" s="3">
-        <v>0</v>
-      </c>
-      <c r="H44" s="2">
-        <v>0</v>
-      </c>
-      <c r="I44" s="3">
-        <v>0</v>
-      </c>
-      <c r="J44" s="4">
-        <v>0</v>
-      </c>
-      <c r="K44" s="3">
-        <v>0</v>
-      </c>
-      <c r="L44" s="4">
-        <v>0</v>
-      </c>
-      <c r="M44" s="4">
-        <v>0</v>
-      </c>
-      <c r="N44" s="3">
-        <v>0</v>
-      </c>
-      <c r="O44" s="4">
-        <v>0</v>
-      </c>
-      <c r="P44" s="3">
+      <c r="G45" s="3">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3">
+        <v>0</v>
+      </c>
+      <c r="J45" s="4">
+        <v>0</v>
+      </c>
+      <c r="K45" s="3">
+        <v>0</v>
+      </c>
+      <c r="L45" s="4">
+        <v>0</v>
+      </c>
+      <c r="M45" s="4">
+        <v>0</v>
+      </c>
+      <c r="N45" s="3">
+        <v>0</v>
+      </c>
+      <c r="O45" s="4">
+        <v>0</v>
+      </c>
+      <c r="P45" s="3">
         <v>2089.4810000000002</v>
       </c>
-      <c r="Q44" s="2">
+      <c r="Q45" s="2">
         <v>153006.82</v>
       </c>
-      <c r="R44" s="4">
-        <v>0</v>
-      </c>
-      <c r="S44" s="4">
-        <v>0</v>
-      </c>
-      <c r="T44" s="4">
-        <v>0</v>
-      </c>
-      <c r="U44" s="4">
-        <v>0</v>
-      </c>
-      <c r="V44" s="4">
-        <v>0</v>
-      </c>
-      <c r="W44" s="4">
+      <c r="R45" s="4">
+        <v>0</v>
+      </c>
+      <c r="S45" s="4">
+        <v>0</v>
+      </c>
+      <c r="T45" s="4">
+        <v>0</v>
+      </c>
+      <c r="U45" s="4">
+        <v>0</v>
+      </c>
+      <c r="V45" s="4">
+        <v>0</v>
+      </c>
+      <c r="W45" s="4">
         <v>10026.299199999999</v>
       </c>
-      <c r="X44" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C45" s="2">
+      <c r="X45" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE45" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="2">
         <v>42725.71</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D46" s="2">
         <v>-8428.67</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E46" s="3">
         <v>655.351</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F46" s="2">
         <v>47989.51</v>
       </c>
-      <c r="P45" s="3">
+      <c r="P46" s="3">
         <v>655.351</v>
       </c>
-      <c r="Q45" s="2">
+      <c r="Q46" s="2">
         <v>47989.51</v>
       </c>
-      <c r="W45" s="4">
+      <c r="W46" s="4">
         <v>3164.87</v>
       </c>
-      <c r="AD45" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C46" s="2">
+      <c r="AD46" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE46" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C47" s="2">
         <v>92629.33</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D47" s="2">
         <v>-19249.41</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E47" s="3">
         <v>1434.13</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F47" s="2">
         <v>105017.31</v>
       </c>
-      <c r="P46" s="3">
+      <c r="P47" s="3">
         <v>1434.13</v>
       </c>
-      <c r="Q46" s="2">
+      <c r="Q47" s="2">
         <v>105017.31</v>
       </c>
-      <c r="W46" s="4">
+      <c r="W47" s="4">
         <v>6861.43</v>
       </c>
-      <c r="AD46" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="AD47" t="s">
         <v>147</v>
       </c>
-      <c r="C47" s="2">
-        <v>-50548.75</v>
-      </c>
-      <c r="D47" s="2">
-        <v>-15631.73</v>
-      </c>
-      <c r="E47" s="3">
-        <v>-425.69799999999998</v>
-      </c>
-      <c r="F47" s="2">
-        <v>-31172.66975495957</v>
-      </c>
-      <c r="G47" s="3">
-        <v>0</v>
-      </c>
-      <c r="H47" s="2">
-        <v>0</v>
-      </c>
-      <c r="I47" s="3">
-        <v>0</v>
-      </c>
-      <c r="J47" s="4">
-        <v>0</v>
-      </c>
-      <c r="K47" s="3">
-        <v>0</v>
-      </c>
-      <c r="L47" s="4">
-        <v>0</v>
-      </c>
-      <c r="M47" s="4">
-        <v>0</v>
-      </c>
-      <c r="N47" s="3">
-        <v>0</v>
-      </c>
-      <c r="O47" s="4">
-        <v>0</v>
-      </c>
-      <c r="P47" s="3">
-        <v>-425.69799999999998</v>
-      </c>
-      <c r="Q47" s="2">
-        <v>-31172.67</v>
-      </c>
-      <c r="R47" s="4">
-        <v>0</v>
-      </c>
-      <c r="S47" s="4">
-        <v>0</v>
-      </c>
-      <c r="T47" s="4">
-        <v>0</v>
-      </c>
-      <c r="U47" s="4">
-        <v>0</v>
-      </c>
-      <c r="V47" s="4">
-        <v>0</v>
-      </c>
-      <c r="W47" s="4">
-        <v>-3744.3519999999999</v>
-      </c>
-      <c r="X47" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z47" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
-        <v>113</v>
+      <c r="AE47" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="C48" s="2">
         <v>-50548.75</v>
@@ -4158,7 +4285,34 @@
         <v>-425.69799999999998</v>
       </c>
       <c r="F48" s="2">
-        <v>-31172.67</v>
+        <v>-31172.66975495957</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <v>0</v>
+      </c>
+      <c r="J48" s="4">
+        <v>0</v>
+      </c>
+      <c r="K48" s="3">
+        <v>0</v>
+      </c>
+      <c r="L48" s="4">
+        <v>0</v>
+      </c>
+      <c r="M48" s="4">
+        <v>0</v>
+      </c>
+      <c r="N48" s="3">
+        <v>0</v>
+      </c>
+      <c r="O48" s="4">
+        <v>0</v>
       </c>
       <c r="P48" s="3">
         <v>-425.69799999999998</v>
@@ -4166,67 +4320,127 @@
       <c r="Q48" s="2">
         <v>-31172.67</v>
       </c>
+      <c r="R48" s="4">
+        <v>0</v>
+      </c>
+      <c r="S48" s="4">
+        <v>0</v>
+      </c>
+      <c r="T48" s="4">
+        <v>0</v>
+      </c>
+      <c r="U48" s="4">
+        <v>0</v>
+      </c>
+      <c r="V48" s="4">
+        <v>0</v>
+      </c>
       <c r="W48" s="4">
+        <v>-3744.3519999999999</v>
+      </c>
+      <c r="X48" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE48" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" s="2">
+        <v>-50548.75</v>
+      </c>
+      <c r="D49" s="2">
+        <v>-15631.73</v>
+      </c>
+      <c r="E49" s="3">
+        <v>-425.69799999999998</v>
+      </c>
+      <c r="F49" s="2">
+        <v>-31172.67</v>
+      </c>
+      <c r="P49" s="3">
+        <v>-425.69799999999998</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>-31172.67</v>
+      </c>
+      <c r="W49" s="4">
         <v>-3744.35</v>
       </c>
-      <c r="AD48" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
+      <c r="AD49" t="s">
         <v>149</v>
       </c>
-      <c r="C49" s="2">
+      <c r="AE49" s="7" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C50" s="2">
         <v>6317922.71</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D50" s="2">
         <v>494174.45</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E50" s="3">
         <v>41554.379000000001</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F50" s="2">
         <v>3042910.53</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I50" s="3">
         <v>4408.0010000000002</v>
       </c>
-      <c r="J49" s="4">
+      <c r="J50" s="4">
         <v>349914.65</v>
       </c>
-      <c r="M49" s="4">
+      <c r="M50" s="4">
         <v>237213.1</v>
       </c>
-      <c r="N49" s="3">
+      <c r="N50" s="3">
         <v>2200.002</v>
       </c>
-      <c r="O49" s="4">
+      <c r="O50" s="4">
         <v>157499.49</v>
       </c>
-      <c r="P49" s="3">
+      <c r="P50" s="3">
         <v>48162.381999999998</v>
       </c>
-      <c r="Q49" s="2">
+      <c r="Q50" s="2">
         <v>3787537.77</v>
       </c>
-      <c r="R49" s="4">
+      <c r="R50" s="4">
         <v>620143.02</v>
       </c>
-      <c r="S49" s="4">
+      <c r="S50" s="4">
         <v>67354.19</v>
       </c>
-      <c r="T49" s="4">
+      <c r="T50" s="4">
         <v>211780.44</v>
       </c>
-      <c r="U49" s="4">
+      <c r="U50" s="4">
         <v>668938.64</v>
       </c>
-      <c r="W49" s="4">
+      <c r="W50" s="4">
         <v>467994.2</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+      <formula1>"Shell &amp; Core, Tenant Improvement, Office, Residential, Parking Garage"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="1.8" right="1.8" top="1.9" bottom="1.9" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Report.py class, avg.py and renamed setup.py to format_file.py
</commit_message>
<xml_diff>
--- a/export1.xlsx
+++ b/export1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stick\Documents\Python\Programs\Excel\ExcelMetrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCACAA6-A0A4-4AC8-A5FC-B38EE2807FD1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBA1B7F-32E6-4A5B-8F68-E9B3CAE2C032}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1380" windowWidth="22155" windowHeight="13800" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="1020" windowWidth="22155" windowHeight="13800" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tblAdditionalInfo" sheetId="1" state="veryHidden" r:id="rId1"/>
@@ -18,20 +18,12 @@
     <sheet name="Bid Breakdown_MetaData" sheetId="3" state="veryHidden" r:id="rId3"/>
     <sheet name="Bid Breakdown" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="154">
   <si>
     <t>tblAdditionalInfo</t>
   </si>
@@ -339,6 +331,9 @@
     <t>Bid Item</t>
   </si>
   <si>
+    <t>Labor $/Hr</t>
+  </si>
+  <si>
     <t>Mat Labor.</t>
   </si>
   <si>
@@ -438,6 +433,9 @@
     <t xml:space="preserve"> || DAS Life Safety System</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
     <t xml:space="preserve"> || Access Control Rough-In</t>
   </si>
   <si>
@@ -484,6 +482,9 @@
   </si>
   <si>
     <t>Revised Totals</t>
+  </si>
+  <si>
+    <t>Office</t>
   </si>
 </sst>
 </file>
@@ -1726,10 +1727,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A2:AE50"/>
+  <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1764,7 +1765,12 @@
     <col min="30" max="30" width="87.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
@@ -1858,10 +1864,13 @@
       <c r="AE2" s="7" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF2" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C3" s="2">
         <v>6266969.3799999999</v>
@@ -1933,13 +1942,15 @@
         <v>0</v>
       </c>
       <c r="AE3" s="7">
-        <f t="shared" ref="AE3:AE49" si="0">D3/I3</f>
-        <v>120.61735920658819</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+        <v>78.774193213494343</v>
+      </c>
+      <c r="AF3" s="7">
+        <v>120.6173592065882</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C4" s="2">
         <v>17718.490000000002</v>
@@ -1984,16 +1995,18 @@
         <v>1312.4</v>
       </c>
       <c r="AD4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE4" s="7">
-        <f t="shared" si="0"/>
-        <v>126.67032063579063</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+        <v>86.043508271915556</v>
+      </c>
+      <c r="AF4" s="7">
+        <v>126.6703206357906</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C5" s="2">
         <v>23082.52</v>
@@ -2038,16 +2051,18 @@
         <v>1709.82</v>
       </c>
       <c r="AD5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE5" s="7">
-        <f t="shared" si="0"/>
-        <v>128.22981888473336</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+        <v>92.610434854451825</v>
+      </c>
+      <c r="AF5" s="7">
+        <v>128.22981888473339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C6" s="2">
         <v>10858.15</v>
@@ -2092,16 +2107,18 @@
         <v>804.31</v>
       </c>
       <c r="AD6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE6" s="7">
-        <f t="shared" si="0"/>
-        <v>121.40286758504358</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+        <v>79.214927383628833</v>
+      </c>
+      <c r="AF6" s="7">
+        <v>121.40286758504359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C7" s="2">
         <v>33420.730000000003</v>
@@ -2146,16 +2163,18 @@
         <v>2475.61</v>
       </c>
       <c r="AD7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE7" s="7">
-        <f t="shared" si="0"/>
-        <v>112.61707006369427</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+        <v>76.396298267884205</v>
+      </c>
+      <c r="AF7" s="7">
+        <v>112.6170700636943</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C8" s="2">
         <v>343502.09</v>
@@ -2203,16 +2222,18 @@
         <v>25444.6</v>
       </c>
       <c r="AD8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE8" s="7">
-        <f t="shared" si="0"/>
-        <v>113.01288864272564</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+        <v>76.465184806425654</v>
+      </c>
+      <c r="AF8" s="7">
+        <v>113.0128886427256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C9" s="2">
         <v>271072.05</v>
@@ -2257,16 +2278,18 @@
         <v>20079.41</v>
       </c>
       <c r="AD9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE9" s="7">
-        <f t="shared" si="0"/>
-        <v>123.44973591855722</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+        <v>80.780436771428015</v>
+      </c>
+      <c r="AF9" s="7">
+        <v>123.4497359185572</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C10" s="2">
         <v>2554.7399999999998</v>
@@ -2311,16 +2334,18 @@
         <v>189.24</v>
       </c>
       <c r="AD10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE10" s="7">
-        <f t="shared" si="0"/>
-        <v>113.70558375634516</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+        <v>76.587175792507196</v>
+      </c>
+      <c r="AF10" s="7">
+        <v>113.70558375634521</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C11" s="2">
         <v>134628.47</v>
@@ -2368,16 +2393,18 @@
         <v>9972.48</v>
       </c>
       <c r="AD11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE11" s="7">
-        <f t="shared" si="0"/>
-        <v>120.93190687659803</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+        <v>78.943207307954879</v>
+      </c>
+      <c r="AF11" s="7">
+        <v>120.93190687659801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C12" s="2">
         <v>13088.93</v>
@@ -2422,16 +2449,18 @@
         <v>969.55</v>
       </c>
       <c r="AD12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE12" s="7">
-        <f t="shared" si="0"/>
-        <v>126.97925939113405</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+        <v>86.975069825178437</v>
+      </c>
+      <c r="AF12" s="7">
+        <v>126.97925939113409</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C13" s="2">
         <v>507457.26</v>
@@ -2476,16 +2505,18 @@
         <v>37589.43</v>
       </c>
       <c r="AD13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE13" s="7">
-        <f t="shared" si="0"/>
-        <v>124.35229494460478</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+        <v>81.764366006479307</v>
+      </c>
+      <c r="AF13" s="7">
+        <v>124.35229494460479</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C14" s="2">
         <v>2926.41</v>
@@ -2530,16 +2561,18 @@
         <v>216.77</v>
       </c>
       <c r="AD14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE14" s="7">
-        <f t="shared" si="0"/>
-        <v>126.43055259227651</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+        <v>85.448853615520278</v>
+      </c>
+      <c r="AF14" s="7">
+        <v>126.4305525922765</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C15" s="2">
         <v>73400.100000000006</v>
@@ -2584,16 +2617,18 @@
         <v>5437.04</v>
       </c>
       <c r="AD15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE15" s="7">
-        <f t="shared" si="0"/>
-        <v>126.80738100843475</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+        <v>86.450630559018833</v>
+      </c>
+      <c r="AF15" s="7">
+        <v>126.8073810084347</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C16" s="2">
         <v>795517.43</v>
@@ -2641,16 +2676,18 @@
         <v>58927.22</v>
       </c>
       <c r="AD16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE16" s="7">
-        <f t="shared" si="0"/>
-        <v>122.62227579070196</v>
-      </c>
-    </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.2">
+        <v>80.058615800311983</v>
+      </c>
+      <c r="AF16" s="7">
+        <v>122.62227579070201</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C17" s="2">
         <v>25277.84</v>
@@ -2695,16 +2732,18 @@
         <v>1872.43</v>
       </c>
       <c r="AD17" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE17" s="7">
-        <f t="shared" si="0"/>
-        <v>121.51630022744504</v>
-      </c>
-    </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.2">
+        <v>79.284730650256009</v>
+      </c>
+      <c r="AF17" s="7">
+        <v>121.516300227445</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C18" s="2">
         <v>118152.69</v>
@@ -2749,16 +2788,18 @@
         <v>8752.0499999999993</v>
       </c>
       <c r="AD18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE18" s="7">
-        <f t="shared" si="0"/>
-        <v>123.99966893583563</v>
-      </c>
-    </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.2">
+        <v>81.350951974992896</v>
+      </c>
+      <c r="AF18" s="7">
+        <v>123.9996689358356</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C19" s="2">
         <v>1486389.63</v>
@@ -2806,16 +2847,18 @@
         <v>110102.94</v>
       </c>
       <c r="AD19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE19" s="7">
-        <f t="shared" si="0"/>
-        <v>112.56560252872298</v>
-      </c>
-    </row>
-    <row r="20" spans="2:31" x14ac:dyDescent="0.2">
+        <v>76.387777476032184</v>
+      </c>
+      <c r="AF19" s="7">
+        <v>112.56560252872301</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C20" s="2">
         <v>154142.46</v>
@@ -2863,16 +2906,18 @@
         <v>11417.96</v>
       </c>
       <c r="AD20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE20" s="7">
-        <f t="shared" si="0"/>
-        <v>121.24534369556478</v>
-      </c>
-    </row>
-    <row r="21" spans="2:31" x14ac:dyDescent="0.2">
+        <v>79.121299918554826</v>
+      </c>
+      <c r="AF20" s="7">
+        <v>121.2453436955648</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C21" s="2">
         <v>651704.13</v>
@@ -2920,16 +2965,18 @@
         <v>48274.38</v>
       </c>
       <c r="AD21" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE21" s="7">
-        <f t="shared" si="0"/>
-        <v>122.86952724285977</v>
-      </c>
-    </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.2">
+        <v>80.259442671447232</v>
+      </c>
+      <c r="AF21" s="7">
+        <v>122.8695272428598</v>
+      </c>
+    </row>
+    <row r="22" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C22" s="2">
         <v>674025.44</v>
@@ -2977,16 +3024,18 @@
         <v>49927.81</v>
       </c>
       <c r="AD22" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE22" s="7">
-        <f t="shared" si="0"/>
-        <v>115.62997852549033</v>
-      </c>
-    </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.2">
+        <v>77.006585760793541</v>
+      </c>
+      <c r="AF22" s="7">
+        <v>115.6299785254903</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C23" s="2">
         <v>34851.06</v>
@@ -3034,16 +3083,18 @@
         <v>2581.56</v>
       </c>
       <c r="AD23" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE23" s="7">
-        <f t="shared" si="0"/>
-        <v>113.54629006949114</v>
-      </c>
-    </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.2">
+        <v>76.562596775518713</v>
+      </c>
+      <c r="AF23" s="7">
+        <v>113.54629006949111</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C24" s="2">
         <v>1471.74</v>
@@ -3088,16 +3139,18 @@
         <v>109.02</v>
       </c>
       <c r="AD24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE24" s="7">
-        <f t="shared" si="0"/>
-        <v>118.86963696369637</v>
-      </c>
-    </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.2">
+        <v>77.994810724502685</v>
+      </c>
+      <c r="AF24" s="7">
+        <v>118.86963696369639</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C25" s="2">
         <v>58762.25</v>
@@ -3145,16 +3198,18 @@
         <v>4352.76</v>
       </c>
       <c r="AD25" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE25" s="7">
-        <f t="shared" si="0"/>
-        <v>120.38070460704608</v>
-      </c>
-    </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.2">
+        <v>78.654322019063997</v>
+      </c>
+      <c r="AF25" s="7">
+        <v>120.3807046070461</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C26" s="2">
         <v>27436.34</v>
@@ -3199,16 +3254,18 @@
         <v>2032.32</v>
       </c>
       <c r="AD26" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE26" s="7">
-        <f t="shared" si="0"/>
-        <v>122.24481299007704</v>
-      </c>
-    </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.2">
+        <v>79.772384378251161</v>
+      </c>
+      <c r="AF26" s="7">
+        <v>122.24481299007699</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C27" s="2">
         <v>6140.51</v>
@@ -3253,16 +3310,18 @@
         <v>454.85</v>
       </c>
       <c r="AD27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE27" s="7">
-        <f t="shared" si="0"/>
-        <v>124.96867469879517</v>
-      </c>
-    </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.2">
+        <v>82.589668783250389</v>
+      </c>
+      <c r="AF27" s="7">
+        <v>124.9686746987952</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C28" s="2">
         <v>7959.05</v>
@@ -3307,16 +3366,18 @@
         <v>589.55999999999995</v>
       </c>
       <c r="AD28" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE28" s="7">
-        <f t="shared" si="0"/>
+        <v>76.93010474893137</v>
+      </c>
+      <c r="AF28" s="7">
         <v>115.3104483211405</v>
       </c>
     </row>
-    <row r="29" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C29" s="2">
         <v>35716.519999999997</v>
@@ -3361,16 +3422,18 @@
         <v>2645.67</v>
       </c>
       <c r="AD29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE29" s="7">
-        <f t="shared" si="0"/>
-        <v>115.78445359311947</v>
-      </c>
-    </row>
-    <row r="30" spans="2:31" x14ac:dyDescent="0.2">
+        <v>77.044125730848023</v>
+      </c>
+      <c r="AF29" s="7">
+        <v>115.78445359311949</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C30" s="2">
         <v>546218.72</v>
@@ -3418,16 +3481,18 @@
         <v>40460.65</v>
       </c>
       <c r="AD30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE30" s="7">
-        <f t="shared" si="0"/>
-        <v>120.06241742220604</v>
-      </c>
-    </row>
-    <row r="31" spans="2:31" x14ac:dyDescent="0.2">
+        <v>78.500083258761464</v>
+      </c>
+      <c r="AF30" s="7">
+        <v>120.062417422206</v>
+      </c>
+    </row>
+    <row r="31" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C31" s="2">
         <v>16306.67</v>
@@ -3472,16 +3537,18 @@
         <v>1207.9000000000001</v>
       </c>
       <c r="AD31" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE31" s="7">
-        <f t="shared" si="0"/>
-        <v>116.07243319268636</v>
-      </c>
-    </row>
-    <row r="32" spans="2:31" x14ac:dyDescent="0.2">
+        <v>77.116099241185211</v>
+      </c>
+      <c r="AF31" s="7">
+        <v>116.0724331926864</v>
+      </c>
+    </row>
+    <row r="32" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C32" s="2">
         <v>1682.46</v>
@@ -3526,16 +3593,18 @@
         <v>124.63</v>
       </c>
       <c r="AD32" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE32" s="7">
-        <f t="shared" si="0"/>
-        <v>124.01159980666988</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+        <v>81.371504660452729</v>
+      </c>
+      <c r="AF32" s="7">
+        <v>124.01159980666991</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C33" s="2">
         <v>28751.22</v>
@@ -3547,16 +3616,18 @@
         <v>2129.7199999999998</v>
       </c>
       <c r="AD33" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE33" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="AE33" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF33" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C34" s="2">
         <v>26898.36</v>
@@ -3601,16 +3672,18 @@
         <v>1992.47</v>
       </c>
       <c r="AD34" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE34" s="7">
-        <f t="shared" si="0"/>
-        <v>112.62091668776907</v>
-      </c>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
+        <v>76.396627105938862</v>
+      </c>
+      <c r="AF34" s="7">
+        <v>112.6209166877691</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C35" s="2">
         <v>16298.61</v>
@@ -3655,16 +3728,18 @@
         <v>1207.3</v>
       </c>
       <c r="AD35" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AE35" s="7">
-        <f t="shared" si="0"/>
-        <v>114.78072651985697</v>
-      </c>
-    </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
+        <v>76.812583782550405</v>
+      </c>
+      <c r="AF35" s="7">
+        <v>114.780726519857</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C36" s="2">
         <v>119556.31</v>
@@ -3676,16 +3751,18 @@
         <v>8856.02</v>
       </c>
       <c r="AD36" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE36" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="AE36" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF36" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C37" s="2">
         <v>120.99</v>
@@ -3756,14 +3833,16 @@
       <c r="Z37" s="5">
         <v>0</v>
       </c>
-      <c r="AE37" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AE37" s="7">
+        <v>73.228285933896998</v>
+      </c>
+      <c r="AF37" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C38" s="2">
         <v>120.99</v>
@@ -3787,16 +3866,18 @@
         <v>8.9600000000000009</v>
       </c>
       <c r="AD38" t="s">
-        <v>139</v>
-      </c>
-      <c r="AE38" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="AE38" s="7">
+        <v>73.228285933896998</v>
+      </c>
+      <c r="AF38" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C39" s="2">
         <v>1011.32</v>
@@ -3867,14 +3948,16 @@
       <c r="Z39" s="5">
         <v>0</v>
       </c>
-      <c r="AE39" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AE39" s="7">
+        <v>73.226911976911992</v>
+      </c>
+      <c r="AF39" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C40" s="2">
         <v>1011.32</v>
@@ -3898,16 +3981,18 @@
         <v>74.91</v>
       </c>
       <c r="AD40" t="s">
-        <v>141</v>
-      </c>
-      <c r="AE40" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="AE40" s="7">
+        <v>73.226911976911992</v>
+      </c>
+      <c r="AF40" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C41" s="2">
         <v>693.46</v>
@@ -3978,14 +4063,16 @@
       <c r="Z41" s="5">
         <v>0</v>
       </c>
-      <c r="AE41" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AE41" s="7">
+        <v>73.227459016393439</v>
+      </c>
+      <c r="AF41" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C42" s="2">
         <v>693.46</v>
@@ -4009,16 +4096,18 @@
         <v>51.37</v>
       </c>
       <c r="AD42" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE42" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="AE42" s="7">
+        <v>73.227459016393439</v>
+      </c>
+      <c r="AF42" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C43" s="2">
         <v>-35678.730000000003</v>
@@ -4089,14 +4178,16 @@
       <c r="Z43" s="5">
         <v>0</v>
       </c>
-      <c r="AE43" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AE43" s="7">
+        <v>73.227184230431646</v>
+      </c>
+      <c r="AF43" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C44" s="2">
         <v>-35678.730000000003</v>
@@ -4120,16 +4211,18 @@
         <v>-2642.87</v>
       </c>
       <c r="AD44" t="s">
-        <v>145</v>
-      </c>
-      <c r="AE44" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="AE44" s="7">
+        <v>73.227184230431646</v>
+      </c>
+      <c r="AF44" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C45" s="2">
         <v>135355.04</v>
@@ -4200,14 +4293,16 @@
       <c r="Z45" s="5">
         <v>0</v>
       </c>
-      <c r="AE45" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AE45" s="7">
+        <v>73.227188952663354</v>
+      </c>
+      <c r="AF45" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C46" s="2">
         <v>42725.71</v>
@@ -4231,16 +4326,18 @@
         <v>3164.87</v>
       </c>
       <c r="AD46" t="s">
-        <v>147</v>
-      </c>
-      <c r="AE46" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="AE46" s="7">
+        <v>73.22718665264874</v>
+      </c>
+      <c r="AF46" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C47" s="2">
         <v>92629.33</v>
@@ -4264,16 +4361,18 @@
         <v>6861.43</v>
       </c>
       <c r="AD47" t="s">
-        <v>147</v>
-      </c>
-      <c r="AE47" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="AE47" s="7">
+        <v>73.227190003695611</v>
+      </c>
+      <c r="AF47" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C48" s="2">
         <v>-50548.75</v>
@@ -4344,14 +4443,16 @@
       <c r="Z48" s="5">
         <v>0</v>
       </c>
-      <c r="AE48" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="49" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="AE48" s="7">
+        <v>73.227193926210603</v>
+      </c>
+      <c r="AF48" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C49" s="2">
         <v>-50548.75</v>
@@ -4375,16 +4476,18 @@
         <v>-3744.35</v>
       </c>
       <c r="AD49" t="s">
-        <v>149</v>
-      </c>
-      <c r="AE49" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="50" spans="2:31" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="AE49" s="7">
+        <v>73.227193926210603</v>
+      </c>
+      <c r="AF49" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C50" s="2">
         <v>6317922.71</v>
@@ -4433,6 +4536,12 @@
       </c>
       <c r="W50" s="4">
         <v>467994.2</v>
+      </c>
+      <c r="AE50">
+        <v>78.640997656635847</v>
+      </c>
+      <c r="AF50">
+        <v>112.1085158555998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>